<commit_message>
Adicionado autodetecção de encoding e correção do template
</commit_message>
<xml_diff>
--- a/output/teste-contas-msc-balver.xlsx
+++ b/output/teste-contas-msc-balver.xlsx
@@ -13,10 +13,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="9">
+  <si>
+    <t>conta_contabil</t>
+  </si>
+  <si>
+    <t>saldo_inicial_valor</t>
+  </si>
+  <si>
+    <t>saldo_inicial_natureza</t>
+  </si>
+  <si>
+    <t>movimento_debito</t>
+  </si>
+  <si>
+    <t>movimento_credito</t>
+  </si>
+  <si>
+    <t>saldo_final_valor</t>
+  </si>
+  <si>
+    <t>saldo_final_natureza</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +80,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +398,904 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>111115000</v>
+      </c>
+      <c r="B2">
+        <v>8745420.67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>713288.4</v>
+      </c>
+      <c r="E2">
+        <v>1176006.65</v>
+      </c>
+      <c r="F2">
+        <v>8282702.42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>111115200</v>
+      </c>
+      <c r="B3">
+        <v>16363.23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>10130.92</v>
+      </c>
+      <c r="E3">
+        <v>1511.62</v>
+      </c>
+      <c r="F3">
+        <v>24982.53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>112410201</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>134183.2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>134183.2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>112619900</v>
+      </c>
+      <c r="B5">
+        <v>633.8099999999999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>933.55</v>
+      </c>
+      <c r="E5">
+        <v>1070.56</v>
+      </c>
+      <c r="F5">
+        <v>496.8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>113819900</v>
+      </c>
+      <c r="B6">
+        <v>75563.2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>65563.2</v>
+      </c>
+      <c r="F6">
+        <v>10000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>114419900</v>
+      </c>
+      <c r="B7">
+        <v>4287433.41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>33954</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>4321387.41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>115610300</v>
+      </c>
+      <c r="B8">
+        <v>201222.98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>82231.69</v>
+      </c>
+      <c r="E8">
+        <v>92775.28999999999</v>
+      </c>
+      <c r="F8">
+        <v>190679.38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>115610400</v>
+      </c>
+      <c r="B9">
+        <v>622502.15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>118979.93</v>
+      </c>
+      <c r="E9">
+        <v>71495.38</v>
+      </c>
+      <c r="F9">
+        <v>669986.7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>115610500</v>
+      </c>
+      <c r="B10">
+        <v>227786.29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>18593.49</v>
+      </c>
+      <c r="E10">
+        <v>36250.39</v>
+      </c>
+      <c r="F10">
+        <v>210129.39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>119110000</v>
+      </c>
+      <c r="B11">
+        <v>12066.23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>2115.97</v>
+      </c>
+      <c r="E11">
+        <v>2442.08</v>
+      </c>
+      <c r="F11">
+        <v>11740.12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>119310000</v>
+      </c>
+      <c r="B12">
+        <v>2487.55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>320</v>
+      </c>
+      <c r="E12">
+        <v>240.41</v>
+      </c>
+      <c r="F12">
+        <v>2567.14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>121110500</v>
+      </c>
+      <c r="B13">
+        <v>23573.45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>133.24</v>
+      </c>
+      <c r="E13">
+        <v>933.55</v>
+      </c>
+      <c r="F13">
+        <v>22773.14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>123110199</v>
+      </c>
+      <c r="B14">
+        <v>48092.01</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>48092.01</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>218911400</v>
+      </c>
+      <c r="B15">
+        <v>43939.04</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>33849.56</v>
+      </c>
+      <c r="E15">
+        <v>28564.1</v>
+      </c>
+      <c r="F15">
+        <v>38653.58</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>218919800</v>
+      </c>
+      <c r="B16">
+        <v>65563.2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>65563.2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>228919800</v>
+      </c>
+      <c r="B17">
+        <v>100000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>100000</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>329910000</v>
+      </c>
+      <c r="B18">
+        <v>138942.43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>75259.89999999999</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>214202.33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>332319900</v>
+      </c>
+      <c r="B19">
+        <v>129289.33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>141450.32</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>270739.65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>351120200</v>
+      </c>
+      <c r="B20">
+        <v>83000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>55000</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>138000</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>352130000</v>
+      </c>
+      <c r="B21">
+        <v>300.69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>300.69</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>352240000</v>
+      </c>
+      <c r="B22">
+        <v>1242402.92</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>405580.3</v>
+      </c>
+      <c r="E22">
+        <v>8688.450000000001</v>
+      </c>
+      <c r="F22">
+        <v>1639294.77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>399130000</v>
+      </c>
+      <c r="B23">
+        <v>38000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>38000</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>399610000</v>
+      </c>
+      <c r="B24">
+        <v>1062.8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>1914.03</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2976.83</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>399910000</v>
+      </c>
+      <c r="B25">
+        <v>3529.2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>3529.2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>412119900</v>
+      </c>
+      <c r="B26">
+        <v>82</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>82</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>412219900</v>
+      </c>
+      <c r="B27">
+        <v>922.2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>159</v>
+      </c>
+      <c r="F27">
+        <v>1081.2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>451120200</v>
+      </c>
+      <c r="B28">
+        <v>83000</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>55000</v>
+      </c>
+      <c r="F28">
+        <v>138000</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>452149900</v>
+      </c>
+      <c r="B29">
+        <v>9274.200000000001</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>9274.200000000001</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>452240000</v>
+      </c>
+      <c r="B30">
+        <v>1963278.83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>15846.11</v>
+      </c>
+      <c r="E30">
+        <v>634027.14</v>
+      </c>
+      <c r="F30">
+        <v>2581459.86</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>463910000</v>
+      </c>
+      <c r="B31">
+        <v>6.97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>6.97</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>712310200</v>
+      </c>
+      <c r="B32">
+        <v>8658025.390000001</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>1032762.25</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>9690787.640000001</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>712319900</v>
+      </c>
+      <c r="B33">
+        <v>1169303.07</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>77500</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1246803.07</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>791130000</v>
+      </c>
+      <c r="B34">
+        <v>388542.25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>388542.25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>791210000</v>
+      </c>
+      <c r="B35">
+        <v>210.02</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>2699.56</v>
+      </c>
+      <c r="E35">
+        <v>2609.58</v>
+      </c>
+      <c r="F35">
+        <v>300</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>812319901</v>
+      </c>
+      <c r="B36">
+        <v>1159675.29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>5237.36</v>
+      </c>
+      <c r="E36">
+        <v>77500</v>
+      </c>
+      <c r="F36">
+        <v>1231937.93</v>
+      </c>
+      <c r="G36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>812319903</v>
+      </c>
+      <c r="B37">
+        <v>9627.780000000001</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>5237.36</v>
+      </c>
+      <c r="F37">
+        <v>14865.14</v>
+      </c>
+      <c r="G37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>821140200</v>
+      </c>
+      <c r="B38">
+        <v>302527.27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>144794.27</v>
+      </c>
+      <c r="F38">
+        <v>447321.54</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>891190000</v>
+      </c>
+      <c r="B39">
+        <v>388542.25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>388542.25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>